<commit_message>
more results, small fix in PQ
</commit_message>
<xml_diff>
--- a/doc/Results/AlexNet_CIFAR10_PS2.xlsx
+++ b/doc/Results/AlexNet_CIFAR10_PS2.xlsx
@@ -1222,11 +1222,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="414912232"/>
-        <c:axId val="414914584"/>
+        <c:axId val="333933648"/>
+        <c:axId val="333934824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="414912232"/>
+        <c:axId val="333933648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14"/>
@@ -1341,12 +1341,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="414914584"/>
+        <c:crossAx val="333934824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="414914584"/>
+        <c:axId val="333934824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.35000000000000003"/>
@@ -1460,7 +1460,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="414912232"/>
+        <c:crossAx val="333933648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1597,7 +1597,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17060282098883978"/>
+          <c:y val="2.3460410557184751E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3024,11 +3031,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="414916152"/>
-        <c:axId val="414913800"/>
+        <c:axId val="333933256"/>
+        <c:axId val="333935608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="414916152"/>
+        <c:axId val="333933256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -3143,12 +3150,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="414913800"/>
+        <c:crossAx val="333935608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="414913800"/>
+        <c:axId val="333935608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -3267,7 +3274,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="414916152"/>
+        <c:crossAx val="333933256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4464,16 +4471,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4497,15 +4504,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4962,7 +4969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:E18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added create_FR_with_different_acc_loss, updates results
</commit_message>
<xml_diff>
--- a/doc/Results/AlexNet_CIFAR10_PS2.xlsx
+++ b/doc/Results/AlexNet_CIFAR10_PS2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summery" sheetId="1" r:id="rId1"/>
@@ -1222,11 +1222,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="333933648"/>
-        <c:axId val="333934824"/>
+        <c:axId val="468190296"/>
+        <c:axId val="468189904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="333933648"/>
+        <c:axId val="468190296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14"/>
@@ -1341,12 +1341,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333934824"/>
+        <c:crossAx val="468189904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="333934824"/>
+        <c:axId val="468189904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.35000000000000003"/>
@@ -1460,7 +1460,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333933648"/>
+        <c:crossAx val="468190296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3031,11 +3031,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="333933256"/>
-        <c:axId val="333935608"/>
+        <c:axId val="468185200"/>
+        <c:axId val="468185592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="333933256"/>
+        <c:axId val="468185200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -3150,12 +3150,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333935608"/>
+        <c:crossAx val="468185592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="333935608"/>
+        <c:axId val="468185592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -3274,7 +3274,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333933256"/>
+        <c:crossAx val="468185200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4969,7 +4969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
@@ -6699,8 +6699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>